<commit_message>
Model Comparision Pipeline Finalisation
</commit_message>
<xml_diff>
--- a/api_estimates.xlsx
+++ b/api_estimates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twoauthentic/Library/CloudStorage/Dropbox/hgupta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BE3D5F-3C86-8E47-91E7-40458FF7BB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26A8709-EDE9-4042-859D-25A17628AB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="760" windowWidth="27600" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -142,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +152,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -189,7 +195,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -895,7 +901,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
@@ -1039,7 +1045,7 @@
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="2">
@@ -1086,7 +1092,7 @@
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="2">
@@ -1133,7 +1139,7 @@
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="2">
@@ -1180,7 +1186,7 @@
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="2">
@@ -1274,7 +1280,7 @@
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="2">
@@ -1368,7 +1374,7 @@
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="2">
@@ -1462,7 +1468,7 @@
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C21" s="2">

</xml_diff>

<commit_message>
Added GPT-5 Pro Pricing
</commit_message>
<xml_diff>
--- a/api_estimates.xlsx
+++ b/api_estimates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twoauthentic/Library/CloudStorage/Dropbox/hgupta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26A8709-EDE9-4042-859D-25A17628AB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25DE761-2DB8-2745-A5DA-FF320F03214F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="760" windowWidth="27600" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="34">
   <si>
     <t>Scenario</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>These enterprise licences provide both access to the underlying AI capabilities and the Microsoft 365 data that Copilot uses. Costs are therefore seat-based rather than per-token.</t>
+  </si>
+  <si>
+    <t>gpt-5 Pro(ChatGPT)</t>
   </si>
 </sst>
 </file>
@@ -500,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1093,7 +1096,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C13" s="2">
         <v>100</v>
@@ -1126,13 +1129,13 @@
         <v>3437200</v>
       </c>
       <c r="M13" s="2">
-        <v>39.08</v>
+        <v>39.078000000000003</v>
       </c>
       <c r="N13" s="2">
-        <v>62.4</v>
+        <v>99.84</v>
       </c>
       <c r="O13" s="2">
-        <v>101.48</v>
+        <v>138.91800000000001</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1140,7 +1143,7 @@
         <v>22</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="2">
         <v>100</v>
@@ -1173,13 +1176,13 @@
         <v>3437200</v>
       </c>
       <c r="M14" s="2">
-        <v>5.21</v>
+        <v>39.08</v>
       </c>
       <c r="N14" s="2">
-        <v>9.98</v>
+        <v>62.4</v>
       </c>
       <c r="O14" s="2">
-        <v>15.19</v>
+        <v>101.48</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1187,7 +1190,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2">
         <v>100</v>
@@ -1220,21 +1223,21 @@
         <v>3437200</v>
       </c>
       <c r="M15" s="2">
-        <v>0.52</v>
+        <v>5.21</v>
       </c>
       <c r="N15" s="2">
-        <v>0.42</v>
+        <v>9.98</v>
       </c>
       <c r="O15" s="2">
-        <v>0.94</v>
+        <v>15.19</v>
       </c>
     </row>
     <row r="16" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>20</v>
+      <c r="B16" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C16" s="2">
         <v>100</v>
@@ -1267,21 +1270,21 @@
         <v>3437200</v>
       </c>
       <c r="M16" s="2">
-        <v>0.73</v>
+        <v>0.52</v>
       </c>
       <c r="N16" s="2">
-        <v>0.35</v>
+        <v>0.42</v>
       </c>
       <c r="O16" s="2">
-        <v>1.08</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="17" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>21</v>
+      <c r="B17" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C17" s="2">
         <v>100</v>
@@ -1327,8 +1330,8 @@
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>25</v>
+      <c r="B18" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C18" s="2">
         <v>100</v>
@@ -1361,21 +1364,21 @@
         <v>3437200</v>
       </c>
       <c r="M18" s="2">
-        <v>2.61</v>
+        <v>0.73</v>
       </c>
       <c r="N18" s="2">
-        <v>0.83</v>
+        <v>0.35</v>
       </c>
       <c r="O18" s="2">
-        <v>3.44</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="19" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>26</v>
+      <c r="B19" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C19" s="2">
         <v>100</v>
@@ -1408,21 +1411,21 @@
         <v>3437200</v>
       </c>
       <c r="M19" s="2">
-        <v>7.82</v>
+        <v>2.61</v>
       </c>
       <c r="N19" s="2">
-        <v>12.48</v>
+        <v>0.83</v>
       </c>
       <c r="O19" s="2">
-        <v>20.3</v>
+        <v>3.44</v>
       </c>
     </row>
     <row r="20" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
+      <c r="B20" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="C20" s="2">
         <v>100</v>
@@ -1455,21 +1458,21 @@
         <v>3437200</v>
       </c>
       <c r="M20" s="2">
-        <v>2.61</v>
+        <v>7.82</v>
       </c>
       <c r="N20" s="2">
-        <v>4.16</v>
+        <v>12.48</v>
       </c>
       <c r="O20" s="2">
-        <v>6.77</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="21" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>28</v>
+      <c r="B21" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C21" s="2">
         <v>100</v>
@@ -1502,60 +1505,60 @@
         <v>3437200</v>
       </c>
       <c r="M21" s="2">
+        <v>2.61</v>
+      </c>
+      <c r="N21" s="2">
+        <v>4.16</v>
+      </c>
+      <c r="O21" s="2">
+        <v>6.77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="2">
+        <v>100</v>
+      </c>
+      <c r="D22" s="2">
+        <v>6</v>
+      </c>
+      <c r="E22" s="2">
+        <v>800</v>
+      </c>
+      <c r="F22" s="2">
+        <v>800</v>
+      </c>
+      <c r="G22" s="2">
+        <v>2</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2">
+        <v>2</v>
+      </c>
+      <c r="J22" s="2">
+        <v>2605200</v>
+      </c>
+      <c r="K22" s="2">
+        <v>832000</v>
+      </c>
+      <c r="L22" s="2">
+        <v>3437200</v>
+      </c>
+      <c r="M22" s="2">
         <v>5.21</v>
       </c>
-      <c r="N21" s="2">
+      <c r="N22" s="2">
         <v>6.66</v>
       </c>
-      <c r="O21" s="2">
+      <c r="O22" s="2">
         <v>11.87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22">
-        <v>100</v>
-      </c>
-      <c r="D22">
-        <v>6</v>
-      </c>
-      <c r="E22">
-        <v>800</v>
-      </c>
-      <c r="F22">
-        <v>800</v>
-      </c>
-      <c r="G22">
-        <v>2</v>
-      </c>
-      <c r="H22">
-        <v>3</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-      <c r="J22">
-        <v>3907800</v>
-      </c>
-      <c r="K22">
-        <v>1248000</v>
-      </c>
-      <c r="L22">
-        <v>5155800</v>
-      </c>
-      <c r="M22">
-        <v>2.46</v>
-      </c>
-      <c r="N22">
-        <v>6.24</v>
-      </c>
-      <c r="O22">
-        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
@@ -1563,7 +1566,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23">
         <v>100</v>
@@ -1596,13 +1599,13 @@
         <v>5155800</v>
       </c>
       <c r="M23">
-        <v>58.62</v>
+        <v>2.46</v>
       </c>
       <c r="N23">
-        <v>93.6</v>
+        <v>6.24</v>
       </c>
       <c r="O23">
-        <v>152.22</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -1610,7 +1613,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24">
         <v>100</v>
@@ -1643,13 +1646,13 @@
         <v>5155800</v>
       </c>
       <c r="M24">
-        <v>7.82</v>
+        <v>58.62</v>
       </c>
       <c r="N24">
-        <v>14.98</v>
+        <v>93.6</v>
       </c>
       <c r="O24">
-        <v>22.79</v>
+        <v>152.22</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
@@ -1657,7 +1660,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25">
         <v>100</v>
@@ -1690,13 +1693,13 @@
         <v>5155800</v>
       </c>
       <c r="M25">
-        <v>0.78</v>
+        <v>7.82</v>
       </c>
       <c r="N25">
-        <v>0.62</v>
+        <v>14.98</v>
       </c>
       <c r="O25">
-        <v>1.41</v>
+        <v>22.79</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -1704,7 +1707,7 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26">
         <v>100</v>
@@ -1737,13 +1740,13 @@
         <v>5155800</v>
       </c>
       <c r="M26">
-        <v>1.0900000000000001</v>
+        <v>0.78</v>
       </c>
       <c r="N26">
-        <v>0.52</v>
+        <v>0.62</v>
       </c>
       <c r="O26">
-        <v>1.62</v>
+        <v>1.41</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
@@ -1751,7 +1754,7 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27">
         <v>100</v>
@@ -1798,7 +1801,7 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C28">
         <v>100</v>
@@ -1831,13 +1834,13 @@
         <v>5155800</v>
       </c>
       <c r="M28">
-        <v>3.91</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="N28">
-        <v>1.25</v>
+        <v>0.52</v>
       </c>
       <c r="O28">
-        <v>5.16</v>
+        <v>1.62</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
@@ -1845,7 +1848,7 @@
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29">
         <v>100</v>
@@ -1878,13 +1881,13 @@
         <v>5155800</v>
       </c>
       <c r="M29">
-        <v>11.72</v>
+        <v>3.91</v>
       </c>
       <c r="N29">
-        <v>18.72</v>
+        <v>1.25</v>
       </c>
       <c r="O29">
-        <v>30.44</v>
+        <v>5.16</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
@@ -1892,7 +1895,7 @@
         <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C30">
         <v>100</v>
@@ -1925,13 +1928,13 @@
         <v>5155800</v>
       </c>
       <c r="M30">
-        <v>3.91</v>
+        <v>11.72</v>
       </c>
       <c r="N30">
-        <v>6.24</v>
+        <v>18.72</v>
       </c>
       <c r="O30">
-        <v>10.15</v>
+        <v>30.44</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
@@ -1939,7 +1942,7 @@
         <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C31">
         <v>100</v>
@@ -1972,21 +1975,21 @@
         <v>5155800</v>
       </c>
       <c r="M31">
-        <v>7.82</v>
+        <v>3.91</v>
       </c>
       <c r="N31">
-        <v>9.98</v>
+        <v>6.24</v>
       </c>
       <c r="O31">
-        <v>17.8</v>
+        <v>10.15</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C32">
         <v>100</v>
@@ -2007,25 +2010,25 @@
         <v>3</v>
       </c>
       <c r="I32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J32">
-        <v>7815600</v>
+        <v>3907800</v>
       </c>
       <c r="K32">
-        <v>2496000</v>
+        <v>1248000</v>
       </c>
       <c r="L32">
-        <v>10311600</v>
+        <v>5155800</v>
       </c>
       <c r="M32">
-        <v>4.92</v>
+        <v>7.82</v>
       </c>
       <c r="N32">
-        <v>12.48</v>
+        <v>9.98</v>
       </c>
       <c r="O32">
-        <v>17.399999999999999</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
@@ -2033,7 +2036,7 @@
         <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C33">
         <v>100</v>
@@ -2066,13 +2069,13 @@
         <v>10311600</v>
       </c>
       <c r="M33">
-        <v>117.23</v>
+        <v>4.92</v>
       </c>
       <c r="N33">
-        <v>187.2</v>
+        <v>12.48</v>
       </c>
       <c r="O33">
-        <v>304.43</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
@@ -2080,7 +2083,7 @@
         <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C34">
         <v>100</v>
@@ -2113,13 +2116,13 @@
         <v>10311600</v>
       </c>
       <c r="M34">
-        <v>15.63</v>
+        <v>117.23</v>
       </c>
       <c r="N34">
-        <v>29.95</v>
+        <v>187.2</v>
       </c>
       <c r="O34">
-        <v>45.58</v>
+        <v>304.43</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
@@ -2127,7 +2130,7 @@
         <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C35">
         <v>100</v>
@@ -2160,13 +2163,13 @@
         <v>10311600</v>
       </c>
       <c r="M35">
-        <v>1.56</v>
+        <v>15.63</v>
       </c>
       <c r="N35">
-        <v>1.25</v>
+        <v>29.95</v>
       </c>
       <c r="O35">
-        <v>2.81</v>
+        <v>45.58</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
@@ -2174,7 +2177,7 @@
         <v>24</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C36">
         <v>100</v>
@@ -2207,13 +2210,13 @@
         <v>10311600</v>
       </c>
       <c r="M36">
-        <v>2.19</v>
+        <v>1.56</v>
       </c>
       <c r="N36">
-        <v>1.05</v>
+        <v>1.25</v>
       </c>
       <c r="O36">
-        <v>3.24</v>
+        <v>2.81</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
@@ -2221,7 +2224,7 @@
         <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C37">
         <v>100</v>
@@ -2268,7 +2271,7 @@
         <v>24</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C38">
         <v>100</v>
@@ -2301,13 +2304,13 @@
         <v>10311600</v>
       </c>
       <c r="M38">
-        <v>7.82</v>
+        <v>2.19</v>
       </c>
       <c r="N38">
-        <v>2.5</v>
+        <v>1.05</v>
       </c>
       <c r="O38">
-        <v>10.31</v>
+        <v>3.24</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
@@ -2315,7 +2318,7 @@
         <v>24</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C39">
         <v>100</v>
@@ -2348,13 +2351,13 @@
         <v>10311600</v>
       </c>
       <c r="M39">
-        <v>23.45</v>
+        <v>7.82</v>
       </c>
       <c r="N39">
-        <v>37.44</v>
+        <v>2.5</v>
       </c>
       <c r="O39">
-        <v>60.89</v>
+        <v>10.31</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
@@ -2362,7 +2365,7 @@
         <v>24</v>
       </c>
       <c r="B40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C40">
         <v>100</v>
@@ -2395,13 +2398,13 @@
         <v>10311600</v>
       </c>
       <c r="M40">
-        <v>7.82</v>
+        <v>23.45</v>
       </c>
       <c r="N40">
-        <v>12.48</v>
+        <v>37.44</v>
       </c>
       <c r="O40">
-        <v>20.3</v>
+        <v>60.89</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
@@ -2409,7 +2412,7 @@
         <v>24</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C41">
         <v>100</v>
@@ -2442,32 +2445,79 @@
         <v>10311600</v>
       </c>
       <c r="M41">
+        <v>7.82</v>
+      </c>
+      <c r="N41">
+        <v>12.48</v>
+      </c>
+      <c r="O41">
+        <v>20.3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42">
+        <v>100</v>
+      </c>
+      <c r="D42">
+        <v>6</v>
+      </c>
+      <c r="E42">
+        <v>800</v>
+      </c>
+      <c r="F42">
+        <v>800</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+      <c r="H42">
+        <v>3</v>
+      </c>
+      <c r="I42">
+        <v>2</v>
+      </c>
+      <c r="J42">
+        <v>7815600</v>
+      </c>
+      <c r="K42">
+        <v>2496000</v>
+      </c>
+      <c r="L42">
+        <v>10311600</v>
+      </c>
+      <c r="M42">
         <v>15.63</v>
       </c>
-      <c r="N41">
+      <c r="N42">
         <v>19.97</v>
       </c>
-      <c r="O41">
+      <c r="O42">
         <v>35.6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>